<commit_message>
Added in substance use cleaning
</commit_message>
<xml_diff>
--- a/metadata/2022/hwb_metadata_s4_su_column_names.xlsx
+++ b/metadata/2022/hwb_metadata_s4_su_column_names.xlsx
@@ -1,23 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\s0196a\ADM-Education-NIF Analysis\Health and Wellbeing Survey\Source\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://scotsconnect-my.sharepoint.com/personal/victoria_dunn_gov_scot/Documents/Git Repos/HWB Rap Project/hwb-census/metadata/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_A902C3CB2582A4CD926B3DCDD7021BC7A767B866" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{104FD54E-461F-4B7C-96C0-FEF61E78B20C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14250"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S4 SU" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -733,7 +745,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -800,42 +812,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1133,17 +1129,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="26.36328125" customWidth="1"/>
-    <col min="2" max="2" width="43.7265625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.7265625" customWidth="1"/>
     <col min="4" max="4" width="15.1796875" customWidth="1"/>
     <col min="5" max="5" width="40.1796875" customWidth="1"/>
@@ -1175,7 +1171,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="13">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1198,1874 +1194,1874 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A3" s="13">
+      <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="13">
+      <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="C4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="5"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" ht="116" x14ac:dyDescent="0.35">
-      <c r="A5" s="13">
+      <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="13">
+      <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="5" t="s">
+      <c r="D6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="13">
+      <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="5" t="s">
+      <c r="C7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="13">
+      <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="5" t="s">
+      <c r="C8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="13">
+      <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="5" t="s">
+      <c r="C9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="13">
+      <c r="A10" s="7">
         <v>9</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="5" t="s">
+      <c r="C10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="13">
+      <c r="A11" s="7">
         <v>10</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="5" t="s">
+      <c r="C11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="13">
+      <c r="A12" s="7">
         <v>11</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="5" t="s">
+      <c r="C12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="13">
+      <c r="A13" s="7">
         <v>12</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="5" t="s">
+      <c r="C13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="13">
+      <c r="A14" s="7">
         <v>13</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="5" t="s">
+      <c r="C14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="13">
+      <c r="A15" s="7">
         <v>14</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="5" t="s">
+      <c r="C15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="13">
+      <c r="A16" s="7">
         <v>15</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="5" t="s">
+      <c r="C16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G16" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="13">
+      <c r="A17" s="7">
         <v>16</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="5" t="s">
+      <c r="C17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G17" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="13">
-        <v>17</v>
-      </c>
-      <c r="B18" s="11" t="s">
+      <c r="A18" s="7">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" s="5" t="s">
+      <c r="C18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="G18" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="13">
+      <c r="A19" s="7">
         <v>18</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" s="5" t="s">
+      <c r="C19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G19" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="13">
+      <c r="A20" s="7">
         <v>19</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" s="5" t="s">
+      <c r="C20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="13">
+      <c r="A21" s="7">
         <v>20</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="5" t="s">
+      <c r="C21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G21" s="5" t="s">
+      <c r="G21" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="13">
+      <c r="A22" s="7">
         <v>21</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E22" s="5" t="s">
+      <c r="C22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F22" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G22" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="13">
-        <v>22</v>
-      </c>
-      <c r="B23" s="11" t="s">
+      <c r="A23" s="7">
+        <v>22</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" s="5" t="s">
+      <c r="C23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="G23" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="13">
+      <c r="A24" s="7">
         <v>23</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E24" s="5" t="s">
+      <c r="C24" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="G24" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="13">
+      <c r="A25" s="7">
         <v>24</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E25" s="5" t="s">
+      <c r="C25" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F25" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="G25" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="13">
+      <c r="A26" s="7">
         <v>25</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E26" s="5" t="s">
+      <c r="D26" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F26" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="G26" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="13">
+      <c r="A27" s="7">
         <v>26</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E27" s="5" t="s">
+      <c r="C27" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="F27" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="G27" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="13">
+      <c r="A28" s="7">
         <v>27</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E28" s="5" t="s">
+      <c r="C28" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="F28" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="G28" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="13">
+      <c r="A29" s="7">
         <v>28</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C29" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E29" s="5" t="s">
+      <c r="C29" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F29" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="G29" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="13">
+      <c r="A30" s="7">
         <v>29</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C30" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E30" s="5" t="s">
+      <c r="C30" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="F30" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="G30" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="13">
+      <c r="A31" s="7">
         <v>30</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C31" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E31" s="5" t="s">
+      <c r="C31" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="F31" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="G31" s="5" t="s">
+      <c r="G31" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="13">
+      <c r="A32" s="7">
         <v>31</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E32" s="5" t="s">
+      <c r="C32" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="F32" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="G32" s="5" t="s">
+      <c r="G32" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="13">
+      <c r="A33" s="7">
         <v>32</v>
       </c>
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C33" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E33" s="5" t="s">
+      <c r="C33" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="F33" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="G33" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="13">
+      <c r="A34" s="7">
         <v>33</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C34" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E34" s="5" t="s">
+      <c r="C34" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="F34" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="G34" s="5" t="s">
+      <c r="G34" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="13">
+      <c r="A35" s="7">
         <v>34</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C35" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E35" s="5" t="s">
+      <c r="C35" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="F35" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="G35" s="5" t="s">
+      <c r="G35" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="13">
+      <c r="A36" s="7">
         <v>35</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="B36" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C36" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E36" s="5" t="s">
+      <c r="C36" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E36" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="F36" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="G36" s="5" t="s">
+      <c r="G36" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="13">
+      <c r="A37" s="7">
         <v>36</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C37" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E37" s="5" t="s">
+      <c r="C37" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F37" s="5" t="s">
+      <c r="F37" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="G37" s="5" t="s">
+      <c r="G37" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="13">
+      <c r="A38" s="7">
         <v>37</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C38" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E38" s="5" t="s">
+      <c r="C38" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F38" s="5" t="s">
+      <c r="F38" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="G38" s="5" t="s">
+      <c r="G38" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="13">
+      <c r="A39" s="7">
         <v>38</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="B39" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C39" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E39" s="5" t="s">
+      <c r="C39" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E39" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F39" s="5" t="s">
+      <c r="F39" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="G39" s="5" t="s">
+      <c r="G39" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="13">
+      <c r="A40" s="7">
         <v>39</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C40" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E40" s="5" t="s">
+      <c r="C40" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E40" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F40" s="5" t="s">
+      <c r="F40" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="G40" s="5" t="s">
+      <c r="G40" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="13">
+      <c r="A41" s="7">
         <v>40</v>
       </c>
-      <c r="B41" s="11" t="s">
+      <c r="B41" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C41" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E41" s="5" t="s">
+      <c r="C41" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F41" s="5" t="s">
+      <c r="F41" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="G41" s="5" t="s">
+      <c r="G41" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="13">
+      <c r="A42" s="7">
         <v>41</v>
       </c>
-      <c r="B42" s="11" t="s">
+      <c r="B42" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C42" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E42" s="5" t="s">
+      <c r="C42" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E42" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F42" s="5" t="s">
+      <c r="F42" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G42" s="5" t="s">
+      <c r="G42" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="13">
+      <c r="A43" s="7">
         <v>42</v>
       </c>
-      <c r="B43" s="11" t="s">
+      <c r="B43" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C43" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E43" s="5" t="s">
+      <c r="C43" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E43" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F43" s="5" t="s">
+      <c r="F43" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="G43" s="5" t="s">
+      <c r="G43" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A44" s="13">
+      <c r="A44" s="7">
         <v>43</v>
       </c>
-      <c r="B44" s="11" t="s">
+      <c r="B44" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C44" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D44" s="8" t="s">
+      <c r="C44" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E44" s="5" t="s">
+      <c r="E44" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F44" s="5" t="s">
+      <c r="F44" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="G44" s="7" t="s">
+      <c r="G44" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="13">
+      <c r="A45" s="7">
         <v>44</v>
       </c>
-      <c r="B45" s="11" t="s">
+      <c r="B45" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C45" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D45" s="8" t="s">
+      <c r="C45" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E45" s="5" t="s">
+      <c r="E45" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="F45" s="5" t="s">
+      <c r="F45" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G45" s="5" t="s">
+      <c r="G45" s="3" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A46" s="13">
+      <c r="A46" s="7">
         <v>45</v>
       </c>
-      <c r="B46" s="11" t="s">
+      <c r="B46" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C46" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D46" s="8" t="s">
+      <c r="C46" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E46" s="5" t="s">
+      <c r="E46" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="F46" s="5" t="s">
+      <c r="F46" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="G46" s="5" t="s">
+      <c r="G46" s="3" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="13">
+      <c r="A47" s="7">
         <v>46</v>
       </c>
-      <c r="B47" s="11" t="s">
+      <c r="B47" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C47" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D47" s="8" t="s">
+      <c r="C47" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E47" s="5" t="s">
+      <c r="E47" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="F47" s="5" t="s">
+      <c r="F47" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="G47" s="5" t="s">
+      <c r="G47" s="3" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A48" s="13">
+      <c r="A48" s="7">
         <v>47</v>
       </c>
-      <c r="B48" s="11" t="s">
+      <c r="B48" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C48" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D48" s="8" t="s">
+      <c r="C48" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D48" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E48" s="5" t="s">
+      <c r="E48" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="F48" s="5" t="s">
+      <c r="F48" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="G48" s="5" t="s">
+      <c r="G48" s="3" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A49" s="13">
+      <c r="A49" s="7">
         <v>48</v>
       </c>
-      <c r="B49" s="11" t="s">
+      <c r="B49" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C49" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D49" s="8" t="s">
+      <c r="C49" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D49" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E49" s="5" t="s">
+      <c r="E49" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="F49" s="5" t="s">
+      <c r="F49" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="G49" s="5" t="s">
+      <c r="G49" s="3" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A50" s="13">
+      <c r="A50" s="7">
         <v>49</v>
       </c>
-      <c r="B50" s="11" t="s">
+      <c r="B50" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C50" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D50" s="8" t="s">
+      <c r="C50" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D50" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E50" s="5" t="s">
+      <c r="E50" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="F50" s="5" t="s">
+      <c r="F50" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="G50" s="5" t="s">
+      <c r="G50" s="3" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A51" s="13">
+      <c r="A51" s="7">
         <v>50</v>
       </c>
-      <c r="B51" s="11" t="s">
+      <c r="B51" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="C51" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D51" s="8" t="s">
+      <c r="C51" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D51" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E51" s="5" t="s">
+      <c r="E51" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="F51" s="5" t="s">
+      <c r="F51" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="G51" s="5" t="s">
+      <c r="G51" s="3" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A52" s="13">
+      <c r="A52" s="7">
         <v>51</v>
       </c>
-      <c r="B52" s="11" t="s">
+      <c r="B52" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="C52" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D52" s="8" t="s">
+      <c r="C52" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D52" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E52" s="5" t="s">
+      <c r="E52" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F52" s="5" t="s">
+      <c r="F52" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="G52" s="5" t="s">
+      <c r="G52" s="3" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A53" s="13">
+      <c r="A53" s="7">
         <v>52</v>
       </c>
-      <c r="B53" s="11" t="s">
+      <c r="B53" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C53" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D53" s="8" t="s">
+      <c r="C53" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D53" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E53" s="5" t="s">
+      <c r="E53" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F53" s="5" t="s">
+      <c r="F53" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="G53" s="5" t="s">
+      <c r="G53" s="3" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A54" s="13">
+      <c r="A54" s="7">
         <v>53</v>
       </c>
-      <c r="B54" s="11" t="s">
+      <c r="B54" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C54" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D54" s="8" t="s">
+      <c r="C54" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D54" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E54" s="5" t="s">
+      <c r="E54" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="F54" s="5" t="s">
+      <c r="F54" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G54" s="5" t="s">
+      <c r="G54" s="3" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A55" s="13">
+      <c r="A55" s="7">
         <v>54</v>
       </c>
-      <c r="B55" s="11" t="s">
+      <c r="B55" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C55" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D55" s="8" t="s">
+      <c r="C55" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D55" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E55" s="5" t="s">
+      <c r="E55" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="F55" s="5" t="s">
+      <c r="F55" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="G55" s="5" t="s">
+      <c r="G55" s="3" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A56" s="13">
+      <c r="A56" s="7">
         <v>55</v>
       </c>
-      <c r="B56" s="11" t="s">
+      <c r="B56" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C56" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D56" s="8" t="s">
+      <c r="C56" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D56" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E56" s="5" t="s">
+      <c r="E56" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="F56" s="5" t="s">
+      <c r="F56" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="G56" s="5" t="s">
+      <c r="G56" s="3" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="13">
+      <c r="A57" s="7">
         <v>56</v>
       </c>
-      <c r="B57" s="11" t="s">
+      <c r="B57" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C57" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D57" s="8" t="s">
+      <c r="C57" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D57" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E57" s="5" t="s">
+      <c r="E57" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="F57" s="5" t="s">
+      <c r="F57" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="G57" s="5" t="s">
+      <c r="G57" s="3" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A58" s="13">
+      <c r="A58" s="7">
         <v>57</v>
       </c>
-      <c r="B58" s="11" t="s">
+      <c r="B58" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C58" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D58" s="8" t="s">
+      <c r="C58" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D58" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E58" s="5" t="s">
+      <c r="E58" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="F58" s="5" t="s">
+      <c r="F58" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="G58" s="5" t="s">
+      <c r="G58" s="3" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A59" s="13">
+      <c r="A59" s="7">
         <v>58</v>
       </c>
-      <c r="B59" s="11" t="s">
+      <c r="B59" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C59" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D59" s="8" t="s">
+      <c r="C59" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D59" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E59" s="5" t="s">
+      <c r="E59" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="F59" s="5" t="s">
+      <c r="F59" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="G59" s="5" t="s">
+      <c r="G59" s="3" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A60" s="13">
+      <c r="A60" s="7">
         <v>59</v>
       </c>
-      <c r="B60" s="11" t="s">
+      <c r="B60" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C60" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D60" s="8" t="s">
+      <c r="C60" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D60" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E60" s="5" t="s">
+      <c r="E60" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="F60" s="5" t="s">
+      <c r="F60" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="G60" s="5" t="s">
+      <c r="G60" s="3" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A61" s="13">
+      <c r="A61" s="7">
         <v>60</v>
       </c>
-      <c r="B61" s="11" t="s">
+      <c r="B61" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="C61" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D61" s="8" t="s">
+      <c r="C61" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D61" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E61" s="5" t="s">
+      <c r="E61" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F61" s="5" t="s">
+      <c r="F61" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="G61" s="5" t="s">
+      <c r="G61" s="3" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A62" s="13">
+      <c r="A62" s="7">
         <v>61</v>
       </c>
-      <c r="B62" s="11" t="s">
+      <c r="B62" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C62" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D62" s="8" t="s">
+      <c r="C62" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D62" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E62" s="5" t="s">
+      <c r="E62" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F62" s="5" t="s">
+      <c r="F62" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="G62" s="5" t="s">
+      <c r="G62" s="3" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A63" s="13">
+      <c r="A63" s="7">
         <v>62</v>
       </c>
-      <c r="B63" s="11" t="s">
+      <c r="B63" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C63" s="5"/>
-      <c r="D63" s="8" t="s">
+      <c r="C63" s="3"/>
+      <c r="D63" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E63" s="5" t="s">
+      <c r="E63" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F63" s="5" t="s">
+      <c r="F63" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="G63" s="7" t="s">
+      <c r="G63" s="4" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A64" s="13">
+      <c r="A64" s="7">
         <v>63</v>
       </c>
-      <c r="B64" s="11" t="s">
+      <c r="B64" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="C64" s="5"/>
-      <c r="D64" s="8" t="s">
+      <c r="C64" s="3"/>
+      <c r="D64" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E64" s="5" t="s">
+      <c r="E64" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F64" s="5" t="s">
+      <c r="F64" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="G64" s="5" t="s">
+      <c r="G64" s="3" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A65" s="13">
+      <c r="A65" s="7">
         <v>64</v>
       </c>
-      <c r="B65" s="11" t="s">
+      <c r="B65" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="C65" s="5"/>
-      <c r="D65" s="8" t="s">
+      <c r="C65" s="3"/>
+      <c r="D65" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E65" s="5" t="s">
+      <c r="E65" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F65" s="5" t="s">
+      <c r="F65" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="G65" s="5" t="s">
+      <c r="G65" s="3" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A66" s="13">
+      <c r="A66" s="7">
         <v>65</v>
       </c>
-      <c r="B66" s="11" t="s">
+      <c r="B66" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="C66" s="5"/>
-      <c r="D66" s="8" t="s">
+      <c r="C66" s="3"/>
+      <c r="D66" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E66" s="5" t="s">
+      <c r="E66" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="F66" s="5" t="s">
+      <c r="F66" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="G66" s="5" t="s">
+      <c r="G66" s="3" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A67" s="13">
+      <c r="A67" s="7">
         <v>66</v>
       </c>
-      <c r="B67" s="11" t="s">
+      <c r="B67" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C67" s="5"/>
-      <c r="D67" s="8" t="s">
+      <c r="C67" s="3"/>
+      <c r="D67" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E67" s="5" t="s">
+      <c r="E67" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="F67" s="5" t="s">
+      <c r="F67" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="G67" s="5" t="s">
+      <c r="G67" s="3" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A68" s="13">
+      <c r="A68" s="7">
         <v>67</v>
       </c>
-      <c r="B68" s="11" t="s">
+      <c r="B68" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="C68" s="5"/>
-      <c r="D68" s="8" t="s">
+      <c r="C68" s="3"/>
+      <c r="D68" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E68" s="5" t="s">
+      <c r="E68" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="F68" s="5" t="s">
+      <c r="F68" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="G68" s="5" t="s">
+      <c r="G68" s="3" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A69" s="13">
+      <c r="A69" s="7">
         <v>68</v>
       </c>
-      <c r="B69" s="11" t="s">
+      <c r="B69" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="C69" s="5"/>
-      <c r="D69" s="8" t="s">
+      <c r="C69" s="3"/>
+      <c r="D69" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E69" s="5" t="s">
+      <c r="E69" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="F69" s="5" t="s">
+      <c r="F69" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="G69" s="5" t="s">
+      <c r="G69" s="3" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A70" s="13">
+      <c r="A70" s="7">
         <v>69</v>
       </c>
-      <c r="B70" s="11" t="s">
+      <c r="B70" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="C70" s="5"/>
-      <c r="D70" s="8" t="s">
+      <c r="C70" s="3"/>
+      <c r="D70" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E70" s="5" t="s">
+      <c r="E70" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="F70" s="5" t="s">
+      <c r="F70" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="G70" s="9" t="s">
+      <c r="G70" s="6" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A71" s="13">
+      <c r="A71" s="7">
         <v>70</v>
       </c>
-      <c r="B71" s="11" t="s">
+      <c r="B71" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="C71" s="5"/>
-      <c r="D71" s="8" t="s">
+      <c r="C71" s="3"/>
+      <c r="D71" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E71" s="5" t="s">
+      <c r="E71" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="F71" s="5" t="s">
+      <c r="F71" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="G71" s="5" t="s">
+      <c r="G71" s="3" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A72" s="13">
+      <c r="A72" s="7">
         <v>71</v>
       </c>
-      <c r="B72" s="11" t="s">
+      <c r="B72" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="C72" s="5"/>
-      <c r="D72" s="8" t="s">
+      <c r="C72" s="3"/>
+      <c r="D72" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E72" s="5" t="s">
+      <c r="E72" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="F72" s="5" t="s">
+      <c r="F72" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="G72" s="5" t="s">
+      <c r="G72" s="3" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A73" s="13">
+      <c r="A73" s="7">
         <v>72</v>
       </c>
-      <c r="B73" s="11" t="s">
+      <c r="B73" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="C73" s="5"/>
-      <c r="D73" s="8" t="s">
+      <c r="C73" s="3"/>
+      <c r="D73" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E73" s="5" t="s">
+      <c r="E73" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="F73" s="5" t="s">
+      <c r="F73" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="G73" s="5" t="s">
+      <c r="G73" s="3" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A74" s="13">
+      <c r="A74" s="7">
         <v>73</v>
       </c>
-      <c r="B74" s="11" t="s">
+      <c r="B74" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="C74" s="5"/>
-      <c r="D74" s="8" t="s">
+      <c r="C74" s="3"/>
+      <c r="D74" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E74" s="5" t="s">
+      <c r="E74" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="F74" s="5" t="s">
+      <c r="F74" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="G74" s="5" t="s">
+      <c r="G74" s="3" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A75" s="13">
+      <c r="A75" s="7">
         <v>74</v>
       </c>
-      <c r="B75" s="11" t="s">
+      <c r="B75" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="C75" s="5"/>
-      <c r="D75" s="8" t="s">
+      <c r="C75" s="3"/>
+      <c r="D75" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E75" s="5" t="s">
+      <c r="E75" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="F75" s="5" t="s">
+      <c r="F75" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="G75" s="5" t="s">
+      <c r="G75" s="3" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A76" s="13">
+      <c r="A76" s="7">
         <v>75</v>
       </c>
-      <c r="B76" s="11" t="s">
+      <c r="B76" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="C76" s="5"/>
-      <c r="D76" s="8" t="s">
+      <c r="C76" s="3"/>
+      <c r="D76" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E76" s="5" t="s">
+      <c r="E76" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="F76" s="5" t="s">
+      <c r="F76" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="G76" s="5" t="s">
+      <c r="G76" s="3" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A77" s="13">
+      <c r="A77" s="7">
         <v>76</v>
       </c>
-      <c r="B77" s="11" t="s">
+      <c r="B77" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="C77" s="5"/>
-      <c r="D77" s="8" t="s">
+      <c r="C77" s="3"/>
+      <c r="D77" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E77" s="5" t="s">
+      <c r="E77" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="F77" s="5" t="s">
+      <c r="F77" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="G77" s="5" t="s">
+      <c r="G77" s="3" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A78" s="13">
+      <c r="A78" s="7">
         <v>77</v>
       </c>
-      <c r="B78" s="11" t="s">
+      <c r="B78" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="C78" s="5"/>
-      <c r="D78" s="8" t="s">
+      <c r="C78" s="3"/>
+      <c r="D78" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E78" s="5" t="s">
+      <c r="E78" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="F78" s="5" t="s">
+      <c r="F78" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="G78" s="5" t="s">
+      <c r="G78" s="3" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A79" s="13">
+      <c r="A79" s="7">
         <v>78</v>
       </c>
-      <c r="B79" s="11" t="s">
+      <c r="B79" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="C79" s="5"/>
-      <c r="D79" s="8" t="s">
+      <c r="C79" s="3"/>
+      <c r="D79" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E79" s="5" t="s">
+      <c r="E79" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="F79" s="5" t="s">
+      <c r="F79" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="G79" s="5" t="s">
+      <c r="G79" s="3" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A80" s="13">
+      <c r="A80" s="7">
         <v>79</v>
       </c>
-      <c r="B80" s="11" t="s">
+      <c r="B80" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="C80" s="5"/>
-      <c r="D80" s="8" t="s">
+      <c r="C80" s="3"/>
+      <c r="D80" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E80" s="5" t="s">
+      <c r="E80" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="F80" s="5" t="s">
+      <c r="F80" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="G80" s="5" t="s">
+      <c r="G80" s="3" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A81" s="13">
+      <c r="A81" s="7">
         <v>80</v>
       </c>
-      <c r="B81" s="11" t="s">
+      <c r="B81" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="C81" s="5"/>
-      <c r="D81" s="8" t="s">
+      <c r="C81" s="3"/>
+      <c r="D81" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E81" s="5" t="s">
+      <c r="E81" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="F81" s="5" t="s">
+      <c r="F81" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="G81" s="5" t="s">
+      <c r="G81" s="3" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A82" s="13">
+      <c r="A82" s="7">
         <v>81</v>
       </c>
-      <c r="B82" s="11" t="s">
+      <c r="B82" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="C82" s="5"/>
-      <c r="D82" s="8" t="s">
+      <c r="C82" s="3"/>
+      <c r="D82" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E82" s="5" t="s">
+      <c r="E82" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="F82" s="5" t="s">
+      <c r="F82" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="G82" s="5" t="s">
+      <c r="G82" s="3" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A83" s="13">
+      <c r="A83" s="7">
         <v>82</v>
       </c>
-      <c r="B83" s="11" t="s">
+      <c r="B83" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="C83" s="5"/>
-      <c r="D83" s="8" t="s">
+      <c r="C83" s="3"/>
+      <c r="D83" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E83" s="5" t="s">
+      <c r="E83" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="F83" s="5" t="s">
+      <c r="F83" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="G83" s="5" t="s">
+      <c r="G83" s="3" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A84" s="13">
+      <c r="A84" s="7">
         <v>83</v>
       </c>
-      <c r="B84" s="11" t="s">
+      <c r="B84" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="C84" s="5"/>
-      <c r="D84" s="8" t="s">
+      <c r="C84" s="3"/>
+      <c r="D84" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E84" s="5" t="s">
+      <c r="E84" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="F84" s="5" t="s">
+      <c r="F84" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="G84" s="5" t="s">
+      <c r="G84" s="3" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A85" s="13">
+      <c r="A85" s="7">
         <v>84</v>
       </c>
-      <c r="B85" s="11" t="s">
+      <c r="B85" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="C85" s="5"/>
-      <c r="D85" s="8" t="s">
+      <c r="C85" s="3"/>
+      <c r="D85" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E85" s="5" t="s">
+      <c r="E85" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="F85" s="5" t="s">
+      <c r="F85" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="G85" s="5" t="s">
+      <c r="G85" s="3" t="s">
         <v>155</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A3 A5 A7 A9 A11 A13 A15 A17 A19 A21 A23 A25 A27 A29 A31 A33 A35 A37 A39 A41 A43 A45 A47 A49 A51 A53 A55 A57 A59 A61 A63 A65 A67 A69 A71 A73 A75 A77 A79 A81 A83 A85">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="FALSE">
+  <conditionalFormatting sqref="A2 A4 A6 A8 A10 A12 A14 A16 A18 A20 A22 A24 A26 A28 A30 A32 A34 A36 A38 A40 A42 A44 A46 A48 A50 A52 A54 A56 A58 A60 A62 A64 A66 A68 A70 A72 A74 A76 A78 A80 A82 A84">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",#REF!)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2 A4 A6 A8 A10 A12 A14 A16 A18 A20 A22 A24 A26 A28 A30 A32 A34 A36 A38 A40 A42 A44 A46 A48 A50 A52 A54 A56 A58 A60 A62 A64 A66 A68 A70 A72 A74 A76 A78 A80 A82 A84">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="FALSE">
+  <conditionalFormatting sqref="A3 A5 A7 A9 A11 A13 A15 A17 A19 A21 A23 A25 A27 A29 A31 A33 A35 A37 A39 A41 A43 A45 A47 A49 A51 A53 A55 A57 A59 A61 A63 A65 A67 A69 A71 A73 A75 A77 A79 A81 A83 A85">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",#REF!)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>